<commit_message>
added graphs for SDI & Electricity
Also renamed datafile to Evan to avoid future conflicts.
</commit_message>
<xml_diff>
--- a/Final Data (1).xlsx
+++ b/Final Data (1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evanlih/Desktop/Github/PUBPOL-543-BEES-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B938E11-8C17-0D47-9C79-BDCB5630FE78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9E86DA-D784-0B4E-8A91-734167596DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -888,8 +888,8 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>